<commit_message>
Modify input schedule using po number and pick by user reference
</commit_message>
<xml_diff>
--- a/backend/src/bin/storages/ppic/PPIC_.xlsx
+++ b/backend/src/bin/storages/ppic/PPIC_.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Tgl Pengajuan</t>
   </si>
@@ -55,127 +55,118 @@
     <t>Ket</t>
   </si>
   <si>
-    <t>08/12/2023</t>
-  </si>
-  <si>
-    <t>KATI KARTIKA MURNI, PT</t>
-  </si>
-  <si>
-    <t>PO20006869</t>
-  </si>
-  <si>
-    <t>3450</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>PKT.062.054187001</t>
-  </si>
-  <si>
-    <t>Karton Tropical Jerry Can 5000ml Pro Vit A New-1</t>
-  </si>
-  <si>
-    <t>28/12/2023</t>
+    <t>13/03/2024</t>
+  </si>
+  <si>
+    <t>CAKRAWALA MEGA INDAH, PT</t>
+  </si>
+  <si>
+    <t>PON23008663</t>
+  </si>
+  <si>
+    <t>2000000</t>
+  </si>
+  <si>
+    <t>4000</t>
+  </si>
+  <si>
+    <t>PET.066.043094003</t>
+  </si>
+  <si>
+    <t>Etiket Shinzu'I [Matsu] 80g HMO+Sakura Ext New 2</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>13/02/2024</t>
-  </si>
-  <si>
-    <t>SINAR PASIFIK LESTARI, PT</t>
-  </si>
-  <si>
-    <t>POF22000100</t>
-  </si>
-  <si>
-    <t>350000</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>EX3.060.512102110</t>
-  </si>
-  <si>
-    <t>MRD B.Logistik - Pelayaran/Ongkos Kapal</t>
-  </si>
-  <si>
-    <t>500</t>
-  </si>
-  <si>
-    <t>06/02/2024</t>
-  </si>
-  <si>
-    <t>POF230100933</t>
-  </si>
-  <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>PKT.062.054168001</t>
-  </si>
-  <si>
-    <t>Karton Tropical Refill 1000ml (EXP) New-1</t>
-  </si>
-  <si>
-    <t>70</t>
-  </si>
-  <si>
-    <t>17/12/2023</t>
-  </si>
-  <si>
-    <t>01/12/2023</t>
-  </si>
-  <si>
-    <t>‭POF23010132‬2</t>
-  </si>
-  <si>
-    <t>1820</t>
-  </si>
-  <si>
-    <t>PKT.062.054169001</t>
-  </si>
-  <si>
-    <t>Karton Tropical Refill 2000ml (EXP) New-1</t>
-  </si>
-  <si>
-    <t>15/12/2023</t>
-  </si>
-  <si>
-    <t>2720</t>
-  </si>
-  <si>
-    <t>PKT.062.054174001</t>
-  </si>
-  <si>
-    <t>Karton Tropical Botol 1000ml Pro Vit A New-1</t>
-  </si>
-  <si>
-    <t>07/02/2024</t>
-  </si>
-  <si>
-    <t>BERKAT SAUDARA GEMILANG, PT</t>
-  </si>
-  <si>
-    <t>PON22000050</t>
-  </si>
-  <si>
-    <t>25000</t>
-  </si>
-  <si>
-    <t>55573</t>
-  </si>
-  <si>
-    <t>PWD.067.047244000</t>
-  </si>
-  <si>
-    <t>Tutup Botol Shinzu'I Ume B.Mist Kokeshi 100ml</t>
-  </si>
-  <si>
-    <t>14/02/2024</t>
+    <t>27/02/2024</t>
+  </si>
+  <si>
+    <t>BUMIMULIA INDAH LESTARI, PT</t>
+  </si>
+  <si>
+    <t>PON24000487</t>
+  </si>
+  <si>
+    <t>170000</t>
+  </si>
+  <si>
+    <t>133558</t>
+  </si>
+  <si>
+    <t>PWD.067.043342001</t>
+  </si>
+  <si>
+    <t>Tube Shinzu'I Facial Wash Snow Mushroom 80ml+20ml + Tutup New</t>
+  </si>
+  <si>
+    <t>30000</t>
+  </si>
+  <si>
+    <t>28/03/2024</t>
+  </si>
+  <si>
+    <t>01/04/2024</t>
+  </si>
+  <si>
+    <t>PON24000854</t>
+  </si>
+  <si>
+    <t>60000</t>
+  </si>
+  <si>
+    <t>PWD.067.043343000</t>
+  </si>
+  <si>
+    <t>Tube Shinzu'I Facial Wash Cica 80ml+20ml + Tutup New</t>
+  </si>
+  <si>
+    <t>21/03/2024</t>
+  </si>
+  <si>
+    <t>25/03/2024</t>
+  </si>
+  <si>
+    <t>25964</t>
+  </si>
+  <si>
+    <t>14/03/2024</t>
+  </si>
+  <si>
+    <t>18/03/2024</t>
+  </si>
+  <si>
+    <t>PLASINDO LESTARI, PT</t>
+  </si>
+  <si>
+    <t>PON24000465</t>
+  </si>
+  <si>
+    <t>130000</t>
+  </si>
+  <si>
+    <t>PPL.067.043143001</t>
+  </si>
+  <si>
+    <t>Plastik Shinzu'I B.Cleanser Refill 85ml [Matsu] New</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>27/03/2024</t>
+  </si>
+  <si>
+    <t>50000</t>
+  </si>
+  <si>
+    <t>27/04/2024</t>
+  </si>
+  <si>
+    <t>70000</t>
+  </si>
+  <si>
+    <t>18/04/2024</t>
   </si>
 </sst>
 </file>
@@ -404,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="80" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -520,7 +511,7 @@
       <c r="N2" s="18"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="29" t="s">
@@ -544,207 +535,359 @@
       <c r="H3" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="29" t="s">
-        <v>21</v>
+      <c r="I3" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="J3" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="B4" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="29" t="s">
+      <c r="B5" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="29" t="s">
+      <c r="B6" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="C6" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="D8" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="E8" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="F8" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="G8" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="H8" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="29" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="29" t="s">
+      <c r="I9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="G5" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" s="29" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="29" t="s">
+      <c r="B10" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="C10" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="29" t="s">
+      <c r="D10" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" s="29" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="29" t="s">
+      <c r="E10" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="29" t="s">
+      <c r="B11" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="G11" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="G12" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="H7" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="J7" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="29" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" s="29" t="s">
+      <c r="H12" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="I12" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="H8" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="J8" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="L8" s="29" t="s">
-        <v>22</v>
+      <c r="J12" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="29" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edit Schedule from table
</commit_message>
<xml_diff>
--- a/backend/src/bin/storages/ppic/PPIC_.xlsx
+++ b/backend/src/bin/storages/ppic/PPIC_.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Tgl Pengajuan</t>
   </si>
@@ -55,19 +55,70 @@
     <t>Ket</t>
   </si>
   <si>
+    <t>27/02/2024</t>
+  </si>
+  <si>
+    <t>BUMIMULIA INDAH LESTARI, PT</t>
+  </si>
+  <si>
+    <t>PON24000487</t>
+  </si>
+  <si>
+    <t>170000</t>
+  </si>
+  <si>
+    <t>133558</t>
+  </si>
+  <si>
+    <t>PWD.067.043342001</t>
+  </si>
+  <si>
+    <t>Tube Shinzu'I Facial Wash Snow Mushroom 80ml+20ml + Tutup New</t>
+  </si>
+  <si>
+    <t>30000</t>
+  </si>
+  <si>
+    <t>28/03/2024</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>01/04/2024</t>
+  </si>
+  <si>
+    <t>PON24000854</t>
+  </si>
+  <si>
+    <t>60000</t>
+  </si>
+  <si>
+    <t>PWD.067.043343000</t>
+  </si>
+  <si>
+    <t>Tube Shinzu'I Facial Wash Cica 80ml+20ml + Tutup New</t>
+  </si>
+  <si>
+    <t>21/03/2024</t>
+  </si>
+  <si>
+    <t>25/03/2024</t>
+  </si>
+  <si>
     <t>13/03/2024</t>
   </si>
   <si>
     <t>CAKRAWALA MEGA INDAH, PT</t>
   </si>
   <si>
-    <t>PON23008663</t>
-  </si>
-  <si>
-    <t>2000000</t>
-  </si>
-  <si>
-    <t>4000</t>
+    <t>PON24000142</t>
+  </si>
+  <si>
+    <t>800000</t>
+  </si>
+  <si>
+    <t>3350000</t>
   </si>
   <si>
     <t>PET.066.043094003</t>
@@ -76,55 +127,7 @@
     <t>Etiket Shinzu'I [Matsu] 80g HMO+Sakura Ext New 2</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>27/02/2024</t>
-  </si>
-  <si>
-    <t>BUMIMULIA INDAH LESTARI, PT</t>
-  </si>
-  <si>
-    <t>PON24000487</t>
-  </si>
-  <si>
-    <t>170000</t>
-  </si>
-  <si>
-    <t>133558</t>
-  </si>
-  <si>
-    <t>PWD.067.043342001</t>
-  </si>
-  <si>
-    <t>Tube Shinzu'I Facial Wash Snow Mushroom 80ml+20ml + Tutup New</t>
-  </si>
-  <si>
-    <t>30000</t>
-  </si>
-  <si>
-    <t>28/03/2024</t>
-  </si>
-  <si>
-    <t>01/04/2024</t>
-  </si>
-  <si>
-    <t>PON24000854</t>
-  </si>
-  <si>
-    <t>60000</t>
-  </si>
-  <si>
-    <t>PWD.067.043343000</t>
-  </si>
-  <si>
-    <t>Tube Shinzu'I Facial Wash Cica 80ml+20ml + Tutup New</t>
-  </si>
-  <si>
-    <t>21/03/2024</t>
-  </si>
-  <si>
-    <t>25/03/2024</t>
+    <t>280000</t>
   </si>
   <si>
     <t>25964</t>
@@ -533,71 +536,71 @@
         <v>20</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="L3" s="29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C4" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="J4" s="29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="L4" s="29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" s="29" t="s">
         <v>26</v>
@@ -609,285 +612,285 @@
         <v>28</v>
       </c>
       <c r="H5" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="J5" s="29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="L5" s="29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="G6" s="29" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="H6" s="29" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="J6" s="29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="L6" s="29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="5" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G7" s="29" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="J7" s="29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="L7" s="29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="G8" s="29" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="H8" s="29" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J8" s="29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="L8" s="29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="H9" s="29" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J9" s="29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="L9" s="29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="5" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F10" s="29" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H10" s="29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J10" s="29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="L10" s="29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="5" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H11" s="29" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J11" s="29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="L11" s="29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="5" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H12" s="29" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J12" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="29" t="s">
         <v>51</v>
-      </c>
-      <c r="J12" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L12" s="29" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update cronjob update,split schedule error count quantity, update login bug while token expired
</commit_message>
<xml_diff>
--- a/backend/src/bin/storages/ppic/PPIC_.xlsx
+++ b/backend/src/bin/storages/ppic/PPIC_.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t>Tgl Pengajuan</t>
   </si>
@@ -67,7 +67,7 @@
     <t>170000</t>
   </si>
   <si>
-    <t>133558</t>
+    <t>103234</t>
   </si>
   <si>
     <t>PWD.067.043342001</t>
@@ -79,97 +79,253 @@
     <t>30000</t>
   </si>
   <si>
-    <t>28/03/2024</t>
+    <t>13/03/2024</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t>PON24000854</t>
+  </si>
+  <si>
+    <t>60000</t>
+  </si>
+  <si>
+    <t>PWD.067.043343000</t>
+  </si>
+  <si>
+    <t>Tube Shinzu'I Facial Wash Cica 80ml+20ml + Tutup New</t>
+  </si>
+  <si>
+    <t>15/03/2024</t>
+  </si>
+  <si>
+    <t>APP PURINUSA EKAPERSADA, PT</t>
+  </si>
+  <si>
+    <t>‭PON24001072‬</t>
+  </si>
+  <si>
+    <t>3000</t>
+  </si>
+  <si>
+    <t>PKT.067.112009000</t>
+  </si>
+  <si>
+    <t>Karton Woshi Woshi Dishwash Refill 200ml x 24pc Promo</t>
+  </si>
+  <si>
     <t>01/04/2024</t>
   </si>
   <si>
-    <t>PON24000854</t>
-  </si>
-  <si>
-    <t>60000</t>
-  </si>
-  <si>
-    <t>PWD.067.043343000</t>
-  </si>
-  <si>
-    <t>Tube Shinzu'I Facial Wash Cica 80ml+20ml + Tutup New</t>
+    <t>20/02/2024</t>
+  </si>
+  <si>
+    <t>‭PON24001074‬</t>
+  </si>
+  <si>
+    <t>4000</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>PKT.067.043104000</t>
+  </si>
+  <si>
+    <t>Karton Shinzu'I B.Cleanser Refill 400mlx24pcs (6V)</t>
+  </si>
+  <si>
+    <t>16/02/2024</t>
+  </si>
+  <si>
+    <t>‭PON24001078‬</t>
+  </si>
+  <si>
+    <t>PKT.067.043044005</t>
+  </si>
+  <si>
+    <t>Karton Shinzu'I B.Lotion 100mlx48pcs(6V) New 4 NS</t>
+  </si>
+  <si>
+    <t>19/03/2024</t>
+  </si>
+  <si>
+    <t>‭PON24001080‬</t>
+  </si>
+  <si>
+    <t>4500</t>
+  </si>
+  <si>
+    <t>PKT.067.043088004</t>
+  </si>
+  <si>
+    <t>Karton Shinzu'I B.Scrub 200grx48pcs (6V) New 4</t>
   </si>
   <si>
     <t>21/03/2024</t>
   </si>
   <si>
-    <t>25/03/2024</t>
-  </si>
-  <si>
-    <t>13/03/2024</t>
-  </si>
-  <si>
-    <t>CAKRAWALA MEGA INDAH, PT</t>
-  </si>
-  <si>
-    <t>PON24000142</t>
-  </si>
-  <si>
-    <t>800000</t>
-  </si>
-  <si>
-    <t>3350000</t>
-  </si>
-  <si>
-    <t>PET.066.043094003</t>
-  </si>
-  <si>
-    <t>Etiket Shinzu'I [Matsu] 80g HMO+Sakura Ext New 2</t>
-  </si>
-  <si>
-    <t>280000</t>
-  </si>
-  <si>
-    <t>25964</t>
-  </si>
-  <si>
-    <t>14/03/2024</t>
+    <t>‭PON24001082‬</t>
+  </si>
+  <si>
+    <t>PKT.067.043045004‬</t>
+  </si>
+  <si>
+    <t>Karton Shinzu'I B.Lotion 210mlx48pcs(6V) New 4</t>
+  </si>
+  <si>
+    <t>02/04/2024</t>
+  </si>
+  <si>
+    <t>04/04/2024</t>
+  </si>
+  <si>
+    <t>‭PON24001084‬</t>
+  </si>
+  <si>
+    <t>09/04/2024</t>
+  </si>
+  <si>
+    <t>PON24001663</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>PKT.067.113002000</t>
+  </si>
+  <si>
+    <t>Karton Garden of Naeem Body Wash 400mlx24pcs</t>
   </si>
   <si>
     <t>18/03/2024</t>
   </si>
   <si>
-    <t>PLASINDO LESTARI, PT</t>
-  </si>
-  <si>
-    <t>PON24000465</t>
-  </si>
-  <si>
-    <t>130000</t>
-  </si>
-  <si>
-    <t>PPL.067.043143001</t>
-  </si>
-  <si>
-    <t>Plastik Shinzu'I B.Cleanser Refill 85ml [Matsu] New</t>
-  </si>
-  <si>
-    <t>10000</t>
+    <t>‭PON24001880</t>
+  </si>
+  <si>
+    <t>02/05/2024</t>
+  </si>
+  <si>
+    <t>‭PON24001881‬</t>
+  </si>
+  <si>
+    <t>PKT.067.103011003</t>
+  </si>
+  <si>
+    <t>Karton ZEN Body Wash Refill 400mlx24pcs New3</t>
   </si>
   <si>
     <t>27/03/2024</t>
   </si>
   <si>
-    <t>50000</t>
-  </si>
-  <si>
-    <t>27/04/2024</t>
-  </si>
-  <si>
-    <t>70000</t>
-  </si>
-  <si>
-    <t>18/04/2024</t>
+    <t>PKT.067.103019002</t>
+  </si>
+  <si>
+    <t>Karton ZEN Body Wash 800ml x 12 New2</t>
+  </si>
+  <si>
+    <t>PKT.067.112008004</t>
+  </si>
+  <si>
+    <t>Karton Woshi Woshi Dishwash Refill 600ml x 12pcs New 3</t>
+  </si>
+  <si>
+    <t>26/03/2024</t>
+  </si>
+  <si>
+    <t>‭PON24001884‬</t>
+  </si>
+  <si>
+    <t>PKT.067.043102000</t>
+  </si>
+  <si>
+    <t>Karton Shinzu'I B.Cleanser 480mlx24pcs (6V)</t>
+  </si>
+  <si>
+    <t>6000</t>
+  </si>
+  <si>
+    <t>PKT.067.043120000</t>
+  </si>
+  <si>
+    <t>Karton Shinzu'I B.Cleanser Refill 800mlx12pcs</t>
+  </si>
+  <si>
+    <t>‭PON24001894‬</t>
+  </si>
+  <si>
+    <t>15/04/2024</t>
+  </si>
+  <si>
+    <t>‭PON24001897‬</t>
+  </si>
+  <si>
+    <t>‭PON24001900‬</t>
+  </si>
+  <si>
+    <t>PKT.067.043105000</t>
+  </si>
+  <si>
+    <t>Karton Shinzu'I B.Cleanser Refill 180mlx48pcs (6V)</t>
+  </si>
+  <si>
+    <t>‭PON24001901‬</t>
+  </si>
+  <si>
+    <t>17/04/2024</t>
+  </si>
+  <si>
+    <t>‭PON24001903‬</t>
+  </si>
+  <si>
+    <t>29/04/2024</t>
+  </si>
+  <si>
+    <t>22/04/2024</t>
+  </si>
+  <si>
+    <t>24/04/2024</t>
+  </si>
+  <si>
+    <t>19/04/2024</t>
+  </si>
+  <si>
+    <t>‭PON24001907‬</t>
+  </si>
+  <si>
+    <t>30/04/2024</t>
+  </si>
+  <si>
+    <t>06/05/2024</t>
+  </si>
+  <si>
+    <t>‭PON24001911‬</t>
+  </si>
+  <si>
+    <t>06/04/2024</t>
+  </si>
+  <si>
+    <t>‭PON24001913‬</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>PKT.067.043106000</t>
+  </si>
+  <si>
+    <t>Karton Shinzu'I B.Cleanser 225mlx48pcs(6V)</t>
+  </si>
+  <si>
+    <t>‭PON24001914‬</t>
+  </si>
+  <si>
+    <t>1400</t>
+  </si>
+  <si>
+    <t>‭PON24001915‬</t>
   </si>
 </sst>
 </file>
@@ -398,7 +554,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="80" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -559,25 +715,25 @@
         <v>15</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F4" s="29" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G4" s="29" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H4" s="29" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J4" s="29" t="s">
         <v>23</v>
@@ -591,31 +747,31 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="5" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="J5" s="29" t="s">
         <v>23</v>
@@ -629,31 +785,31 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="5" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="G6" s="29" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="H6" s="29" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="J6" s="29" t="s">
         <v>23</v>
@@ -667,31 +823,31 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="5" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="G7" s="29" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="J7" s="29" t="s">
         <v>23</v>
@@ -705,31 +861,31 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="5" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="G8" s="29" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="H8" s="29" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="J8" s="29" t="s">
         <v>23</v>
@@ -743,31 +899,31 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="5" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="H9" s="29" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="J9" s="29" t="s">
         <v>23</v>
@@ -781,31 +937,31 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="5" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F10" s="29" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H10" s="29" t="s">
         <v>47</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="J10" s="29" t="s">
         <v>23</v>
@@ -819,31 +975,31 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="5" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H11" s="29" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="J11" s="29" t="s">
         <v>23</v>
@@ -857,40 +1013,1066 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="G12" s="29" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="H12" s="29" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="I12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J12" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="J12" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L12" s="29" t="s">
-        <v>51</v>
+      <c r="G13" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J13" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J15" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H16" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J16" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J17" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L17" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="H18" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J18" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L18" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L19" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="H20" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J20" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L20" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="G21" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="H21" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J21" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L21" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="G22" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="H22" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J22" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L22" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="G23" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="H23" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="J23" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L23" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J24" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L24" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="H25" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J25" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L25" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="G26" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="H26" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L26" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="H27" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J27" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L27" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="F28" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="G28" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="H28" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J28" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L28" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H29" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J29" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L29" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="F30" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="H30" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="J30" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L30" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="G31" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="H31" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="J31" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L31" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="F32" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="G32" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="H32" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="J32" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L32" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="F33" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="G33" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="H33" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J33" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L33" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="G34" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="H34" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="J34" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L34" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F35" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="G35" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="H35" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="J35" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L35" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F36" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="G36" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="H36" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="J36" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L36" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="F37" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="G37" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="H37" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J37" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L37" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="E38" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="F38" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="G38" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="H38" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J38" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L38" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B39" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E39" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="F39" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="G39" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="H39" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J39" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L39" s="29" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>